<commit_message>
Working on selecting best pruned tree
</commit_message>
<xml_diff>
--- a/RegimeShiftsSpecies.xlsx
+++ b/RegimeShiftsSpecies.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
   <si>
     <t>Rigime shift results:</t>
   </si>
@@ -192,6 +192,9 @@
   </si>
   <si>
     <t>Blackbelly rosefish</t>
+  </si>
+  <si>
+    <t>n splits for lowest xerror</t>
   </si>
 </sst>
 </file>
@@ -517,471 +520,504 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="17.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>43</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>45</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>44</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>45</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>47</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>45</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>54</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>2000</v>
       </c>
-      <c r="C3" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>2000</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>2011</v>
       </c>
-      <c r="E4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="C6">
         <v>2003</v>
       </c>
-      <c r="C6" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="D6" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
         <v>49</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="B8">
+      <c r="C8">
         <v>1992</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8">
+      <c r="D8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8">
         <v>1995</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>50</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>2009</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B9" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="C9">
         <v>1999</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>2011</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>2016</v>
       </c>
-      <c r="G9" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
         <v>51</v>
       </c>
-      <c r="B10">
+      <c r="C10">
         <v>1995</v>
       </c>
-      <c r="C10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10">
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10">
         <v>2011</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10">
+        <v>2012</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A11">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11">
+        <v>2011</v>
+      </c>
+      <c r="D11" t="s">
         <v>50</v>
       </c>
-      <c r="F10">
+      <c r="E11">
+        <v>2018</v>
+      </c>
+      <c r="G11">
+        <v>2016</v>
+      </c>
+      <c r="I11">
+        <v>2013</v>
+      </c>
+      <c r="K11">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>0</v>
+      </c>
+      <c r="B12" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12">
+        <v>1995</v>
+      </c>
+      <c r="D12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12">
+        <v>2005</v>
+      </c>
+      <c r="G12">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13">
+        <v>2008</v>
+      </c>
+      <c r="D13" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13">
         <v>2012</v>
       </c>
-      <c r="G10" t="s">
+      <c r="F13" t="s">
+        <v>46</v>
+      </c>
+      <c r="G13">
+        <v>2019</v>
+      </c>
+      <c r="H13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I13">
+        <v>2006</v>
+      </c>
+      <c r="J13" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14">
+        <v>2016</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15">
+        <v>2006</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15">
+        <v>2012</v>
+      </c>
+      <c r="F15" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11">
-        <v>2011</v>
-      </c>
-      <c r="C11" t="s">
+      <c r="G15">
+        <v>2019</v>
+      </c>
+      <c r="H15" t="s">
         <v>50</v>
       </c>
-      <c r="D11">
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16">
+        <v>2000</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16">
+        <v>2008</v>
+      </c>
+      <c r="F16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>2</v>
+      </c>
+      <c r="B17" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17">
+        <v>1998</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17">
         <v>2016</v>
       </c>
-      <c r="F11">
-        <v>2018</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12">
-        <v>1995</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="F17" t="s">
         <v>50</v>
       </c>
-      <c r="D12">
-        <v>2005</v>
-      </c>
-      <c r="F12">
-        <v>2017</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13">
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18">
+        <v>2000</v>
+      </c>
+      <c r="E18">
         <v>2008</v>
       </c>
-      <c r="C13" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13">
-        <v>2012</v>
-      </c>
-      <c r="E13" t="s">
-        <v>46</v>
-      </c>
-      <c r="F13">
-        <v>2019</v>
-      </c>
-      <c r="G13" t="s">
-        <v>46</v>
-      </c>
-      <c r="I13" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>9</v>
-      </c>
-      <c r="B14">
-        <v>2016</v>
-      </c>
-      <c r="C14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>55</v>
-      </c>
-      <c r="B15">
-        <v>2006</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15">
-        <v>2012</v>
-      </c>
-      <c r="E15" t="s">
+      <c r="F18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19">
+        <v>2000</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19">
+        <v>2010</v>
+      </c>
+      <c r="F19" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B22" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B24" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>20</v>
+      </c>
+      <c r="C26">
+        <v>2002</v>
+      </c>
+      <c r="D26" t="s">
         <v>50</v>
       </c>
-      <c r="F15">
-        <v>2019</v>
-      </c>
-      <c r="G15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B16">
-        <v>2000</v>
-      </c>
-      <c r="C16" t="s">
-        <v>46</v>
-      </c>
-      <c r="D16">
-        <v>2008</v>
-      </c>
-      <c r="E16" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>11</v>
-      </c>
-      <c r="B17">
-        <v>1998</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17">
-        <v>2016</v>
-      </c>
-      <c r="E17" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18">
-        <v>2000</v>
-      </c>
-      <c r="D18">
-        <v>2008</v>
-      </c>
-      <c r="E18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19">
-        <v>2000</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19">
-        <v>2010</v>
-      </c>
-      <c r="E19" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
-        <v>20</v>
-      </c>
-      <c r="B26">
-        <v>2002</v>
-      </c>
-      <c r="C26" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B27" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B28" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B30" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B31" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B32" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B33" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B35" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B36" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B37" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B38" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B39" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B40" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B41" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B42" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B43" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B44" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A45" t="s">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B45" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A46" t="s">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B46" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A47" t="s">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B47" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test for single species regime splits
</commit_message>
<xml_diff>
--- a/RegimeShiftsSpecies.xlsx
+++ b/RegimeShiftsSpecies.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
   <si>
     <t>Rigime shift results:</t>
   </si>
@@ -195,6 +195,9 @@
   </si>
   <si>
     <t>n splits for lowest xerror</t>
+  </si>
+  <si>
+    <t>Cusk</t>
   </si>
 </sst>
 </file>
@@ -520,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K47"/>
+  <dimension ref="A1:K48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -876,148 +879,213 @@
       <c r="B20" t="s">
         <v>14</v>
       </c>
+      <c r="C20" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>0</v>
+      </c>
       <c r="B21" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B22" t="s">
+      <c r="C22">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>0</v>
+      </c>
+      <c r="B23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B23" t="s">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B24" t="s">
+      <c r="C24">
+        <v>2012</v>
+      </c>
+      <c r="E24">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>0</v>
+      </c>
+      <c r="B25" t="s">
         <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B25" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
+        <v>2</v>
+      </c>
+      <c r="B26" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26">
+        <v>1999</v>
+      </c>
+      <c r="E26">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A27">
         <v>1</v>
       </c>
-      <c r="B26" t="s">
+      <c r="B27" t="s">
         <v>20</v>
       </c>
-      <c r="C26">
+      <c r="C27">
         <v>2002</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D27" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B27" t="s">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B28" t="s">
+      <c r="C28">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>2</v>
+      </c>
+      <c r="B29" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B29" t="s">
+      <c r="C29">
+        <v>2000</v>
+      </c>
+      <c r="E29">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>2</v>
+      </c>
+      <c r="B30" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="B30" t="s">
-        <v>24</v>
+      <c r="C30">
+        <v>2010</v>
+      </c>
+      <c r="E30">
+        <v>2000</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="35" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="36" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="37" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="38" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="39" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="42" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="43" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="44" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="46" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B48" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added in splits 4 and 5
</commit_message>
<xml_diff>
--- a/RegimeShiftsSpecies.xlsx
+++ b/RegimeShiftsSpecies.xlsx
@@ -12,7 +12,10 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Results" sheetId="1" r:id="rId1"/>
+    <sheet name="RegimeChangeSpp" sheetId="4" r:id="rId2"/>
+    <sheet name="2000" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="60">
   <si>
     <t>Rigime shift results:</t>
   </si>
@@ -198,6 +201,12 @@
   </si>
   <si>
     <t>Cusk</t>
+  </si>
+  <si>
+    <t>Spot</t>
+  </si>
+  <si>
+    <t>Condition drop after 2000</t>
   </si>
 </sst>
 </file>
@@ -523,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K48"/>
+  <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -783,7 +792,7 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B15" t="s">
         <v>55</v>
@@ -824,7 +833,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>2</v>
       </c>
@@ -844,7 +853,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>12</v>
       </c>
@@ -858,7 +867,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>13</v>
       </c>
@@ -875,7 +884,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>14</v>
       </c>
@@ -883,7 +892,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>0</v>
       </c>
@@ -891,7 +900,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>1</v>
       </c>
@@ -902,7 +911,7 @@
         <v>2012</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>0</v>
       </c>
@@ -910,7 +919,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>2</v>
       </c>
@@ -924,7 +933,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>0</v>
       </c>
@@ -932,7 +941,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>2</v>
       </c>
@@ -946,7 +955,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>1</v>
       </c>
@@ -960,7 +969,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>1</v>
       </c>
@@ -971,7 +980,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>2</v>
       </c>
@@ -985,7 +994,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>2</v>
       </c>
@@ -999,97 +1008,1359 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>1</v>
+      </c>
       <c r="B31" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C31">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>5</v>
+      </c>
       <c r="B32" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C32">
+        <v>2002</v>
+      </c>
+      <c r="E32">
+        <v>2019</v>
+      </c>
+      <c r="G32">
+        <v>2001</v>
+      </c>
+      <c r="I32">
+        <v>1998</v>
+      </c>
+      <c r="K32">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>1</v>
+      </c>
       <c r="B33" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C33">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>1</v>
+      </c>
       <c r="B34" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C34">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>1</v>
+      </c>
       <c r="B35" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C35">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>3</v>
+      </c>
       <c r="B36" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C36">
+        <v>2007</v>
+      </c>
+      <c r="E36">
+        <v>2011</v>
+      </c>
+      <c r="G36">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>1</v>
+      </c>
       <c r="B37" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="C37">
+        <v>2000</v>
+      </c>
+      <c r="E37">
+        <v>2019</v>
+      </c>
+      <c r="G37">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>0</v>
+      </c>
       <c r="B38" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>3</v>
+      </c>
       <c r="B39" t="s">
+        <v>58</v>
+      </c>
+      <c r="C39">
+        <v>2013</v>
+      </c>
+      <c r="E39">
+        <v>2004</v>
+      </c>
+      <c r="G39">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B40" t="s">
+      <c r="C40">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B41" t="s">
+      <c r="C41">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B42" t="s">
+      <c r="C42">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43">
+        <v>2</v>
+      </c>
+      <c r="B43" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B43" t="s">
+      <c r="C43">
+        <v>2003</v>
+      </c>
+      <c r="E43">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44">
+        <v>0</v>
+      </c>
+      <c r="B44" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B44" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45">
+        <v>0</v>
+      </c>
+      <c r="B45" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B45" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B46" t="s">
+      <c r="C46">
+        <v>2012</v>
+      </c>
+      <c r="E46">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47">
+        <v>4</v>
+      </c>
+      <c r="B47" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B47" t="s">
+      <c r="C47">
+        <v>2019</v>
+      </c>
+      <c r="E47">
+        <v>2009</v>
+      </c>
+      <c r="G47">
+        <v>2012</v>
+      </c>
+      <c r="I47">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48">
+        <v>1</v>
+      </c>
+      <c r="B48" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B48" t="s">
+      <c r="C48">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>1</v>
+      </c>
+      <c r="B49" t="s">
         <v>41</v>
+      </c>
+      <c r="C49">
+        <v>2001</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K40"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" t="s">
+        <v>45</v>
+      </c>
+      <c r="I2" t="s">
+        <v>54</v>
+      </c>
+      <c r="J2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2000</v>
+      </c>
+      <c r="D3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>2000</v>
+      </c>
+      <c r="E4">
+        <v>2011</v>
+      </c>
+      <c r="F4" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>2003</v>
+      </c>
+      <c r="D5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6">
+        <v>1992</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6">
+        <v>1995</v>
+      </c>
+      <c r="F6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G6">
+        <v>2009</v>
+      </c>
+      <c r="H6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>1999</v>
+      </c>
+      <c r="E7">
+        <v>2011</v>
+      </c>
+      <c r="G7">
+        <v>2016</v>
+      </c>
+      <c r="H7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C8">
+        <v>1995</v>
+      </c>
+      <c r="D8" t="s">
+        <v>50</v>
+      </c>
+      <c r="E8">
+        <v>2011</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G8">
+        <v>2012</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+      <c r="C9">
+        <v>2011</v>
+      </c>
+      <c r="D9" t="s">
+        <v>50</v>
+      </c>
+      <c r="E9">
+        <v>2018</v>
+      </c>
+      <c r="G9">
+        <v>2016</v>
+      </c>
+      <c r="I9">
+        <v>2013</v>
+      </c>
+      <c r="K9">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10">
+        <v>1995</v>
+      </c>
+      <c r="D10" t="s">
+        <v>50</v>
+      </c>
+      <c r="E10">
+        <v>2005</v>
+      </c>
+      <c r="G10">
+        <v>2017</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>2008</v>
+      </c>
+      <c r="D11" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11">
+        <v>2012</v>
+      </c>
+      <c r="F11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G11">
+        <v>2019</v>
+      </c>
+      <c r="H11" t="s">
+        <v>46</v>
+      </c>
+      <c r="I11">
+        <v>2006</v>
+      </c>
+      <c r="J11" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>2016</v>
+      </c>
+      <c r="D12" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+      <c r="C13">
+        <v>2006</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E13">
+        <v>2012</v>
+      </c>
+      <c r="F13" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13">
+        <v>2019</v>
+      </c>
+      <c r="H13" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B14" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14">
+        <v>2000</v>
+      </c>
+      <c r="D14" t="s">
+        <v>46</v>
+      </c>
+      <c r="E14">
+        <v>2008</v>
+      </c>
+      <c r="F14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15">
+        <v>1998</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E15">
+        <v>2016</v>
+      </c>
+      <c r="F15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16">
+        <v>2000</v>
+      </c>
+      <c r="E16">
+        <v>2008</v>
+      </c>
+      <c r="F16" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17">
+        <v>2000</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E17">
+        <v>2010</v>
+      </c>
+      <c r="F17" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19">
+        <v>2012</v>
+      </c>
+      <c r="E19">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>19</v>
+      </c>
+      <c r="C20">
+        <v>1999</v>
+      </c>
+      <c r="E20">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21">
+        <v>2002</v>
+      </c>
+      <c r="D21" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>21</v>
+      </c>
+      <c r="C22">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>2</v>
+      </c>
+      <c r="B23" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23">
+        <v>2000</v>
+      </c>
+      <c r="E23">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24">
+        <v>2010</v>
+      </c>
+      <c r="E24">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26">
+        <v>2002</v>
+      </c>
+      <c r="E26">
+        <v>2019</v>
+      </c>
+      <c r="G26">
+        <v>2001</v>
+      </c>
+      <c r="I26">
+        <v>1998</v>
+      </c>
+      <c r="K26">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A30">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>29</v>
+      </c>
+      <c r="C30">
+        <v>2007</v>
+      </c>
+      <c r="E30">
+        <v>2011</v>
+      </c>
+      <c r="G30">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31" t="s">
+        <v>30</v>
+      </c>
+      <c r="C31">
+        <v>2000</v>
+      </c>
+      <c r="E31">
+        <v>2019</v>
+      </c>
+      <c r="G31">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A32">
+        <v>3</v>
+      </c>
+      <c r="B32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C32">
+        <v>2013</v>
+      </c>
+      <c r="E32">
+        <v>2004</v>
+      </c>
+      <c r="G32">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33" t="s">
+        <v>32</v>
+      </c>
+      <c r="C33">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34" t="s">
+        <v>33</v>
+      </c>
+      <c r="C34">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C35">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36">
+        <v>2</v>
+      </c>
+      <c r="B36" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36">
+        <v>2003</v>
+      </c>
+      <c r="E36">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37">
+        <v>2</v>
+      </c>
+      <c r="B37" t="s">
+        <v>38</v>
+      </c>
+      <c r="C37">
+        <v>2012</v>
+      </c>
+      <c r="E37">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38">
+        <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>39</v>
+      </c>
+      <c r="C38">
+        <v>2019</v>
+      </c>
+      <c r="E38">
+        <v>2009</v>
+      </c>
+      <c r="G38">
+        <v>2012</v>
+      </c>
+      <c r="I38">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39" t="s">
+        <v>40</v>
+      </c>
+      <c r="C39">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40">
+        <v>2001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="17.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4">
+        <v>2000</v>
+      </c>
+      <c r="E4">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5">
+        <v>2003</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>1999</v>
+      </c>
+      <c r="E6">
+        <v>2011</v>
+      </c>
+      <c r="F6">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7">
+        <v>2011</v>
+      </c>
+      <c r="E7">
+        <v>2018</v>
+      </c>
+      <c r="F7">
+        <v>2016</v>
+      </c>
+      <c r="G7">
+        <v>2013</v>
+      </c>
+      <c r="H7">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8">
+        <v>2000</v>
+      </c>
+      <c r="E8">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>2</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9">
+        <v>1998</v>
+      </c>
+      <c r="E9">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10">
+        <v>2000</v>
+      </c>
+      <c r="E10">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>13</v>
+      </c>
+      <c r="D11">
+        <v>2000</v>
+      </c>
+      <c r="E11">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12">
+        <v>2012</v>
+      </c>
+      <c r="E12">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>2</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D13">
+        <v>1999</v>
+      </c>
+      <c r="E13">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C14" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14">
+        <v>2002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15">
+        <v>2000</v>
+      </c>
+      <c r="E15">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>2</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16">
+        <v>2010</v>
+      </c>
+      <c r="E16">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>5</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17">
+        <v>2002</v>
+      </c>
+      <c r="E17">
+        <v>2019</v>
+      </c>
+      <c r="F17">
+        <v>2001</v>
+      </c>
+      <c r="G17">
+        <v>1998</v>
+      </c>
+      <c r="H17">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>1</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>1</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20">
+        <v>2000</v>
+      </c>
+      <c r="E20">
+        <v>2019</v>
+      </c>
+      <c r="F20">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>3</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D21">
+        <v>2013</v>
+      </c>
+      <c r="E21">
+        <v>2004</v>
+      </c>
+      <c r="F21">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
+        <v>32</v>
+      </c>
+      <c r="D22">
+        <v>1996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23" t="s">
+        <v>33</v>
+      </c>
+      <c r="D23">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>2</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
+        <v>35</v>
+      </c>
+      <c r="D24">
+        <v>2003</v>
+      </c>
+      <c r="E24">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A25">
+        <v>2</v>
+      </c>
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" t="s">
+        <v>38</v>
+      </c>
+      <c r="D25">
+        <v>2012</v>
+      </c>
+      <c r="E25">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C26" t="s">
+        <v>41</v>
+      </c>
+      <c r="D26">
+        <v>2001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added total copepod regime shifts from Harvey, by season
</commit_message>
<xml_diff>
--- a/RegimeShiftsSpecies.xlsx
+++ b/RegimeShiftsSpecies.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7050" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="1" r:id="rId1"/>
     <sheet name="RegimeChangeSpp" sheetId="4" r:id="rId2"/>
     <sheet name="2000" sheetId="5" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="2010" sheetId="6" r:id="rId4"/>
+    <sheet name="Environmental changes" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="290" uniqueCount="78">
   <si>
     <t>Rigime shift results:</t>
   </si>
@@ -207,6 +208,60 @@
   </si>
   <si>
     <t>Condition drop after 2000</t>
+  </si>
+  <si>
+    <t>Index</t>
+  </si>
+  <si>
+    <t>Total copepods</t>
+  </si>
+  <si>
+    <t>Sm/lg copepods</t>
+  </si>
+  <si>
+    <t>spring temp</t>
+  </si>
+  <si>
+    <t>summer temp</t>
+  </si>
+  <si>
+    <t>fall temp</t>
+  </si>
+  <si>
+    <t>winter temp</t>
+  </si>
+  <si>
+    <t>fall bloom mag</t>
+  </si>
+  <si>
+    <t>fall bloom duration</t>
+  </si>
+  <si>
+    <t>Year changes after</t>
+  </si>
+  <si>
+    <t>Increase after 2010</t>
+  </si>
+  <si>
+    <t>main index that decreased in 2000, increased again in 2010</t>
+  </si>
+  <si>
+    <t>higher temps after 2009</t>
+  </si>
+  <si>
+    <t>higher temps after 2010</t>
+  </si>
+  <si>
+    <t>higher temps after 2011</t>
+  </si>
+  <si>
+    <t>outlier high copepods in 1996, increased copepods after 2014 especially in GOM</t>
+  </si>
+  <si>
+    <t>low temps from 2002-2004 or 2005, increased temps after 2009</t>
+  </si>
+  <si>
+    <t>Small/large copepod decline in 2000 aligns with condition declines</t>
   </si>
 </sst>
 </file>
@@ -534,8 +589,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -543,7 +598,7 @@
     <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -551,7 +606,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -583,7 +638,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -594,7 +649,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -608,7 +663,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>4</v>
       </c>
@@ -616,7 +671,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>5</v>
       </c>
@@ -627,7 +682,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>49</v>
       </c>
@@ -635,7 +690,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>3</v>
       </c>
@@ -661,7 +716,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>7</v>
       </c>
@@ -678,35 +733,23 @@
         <v>46</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="1">
-        <v>2</v>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="A10">
+        <v>1</v>
       </c>
       <c r="B10" t="s">
         <v>51</v>
       </c>
       <c r="C10">
-        <v>1995</v>
+        <v>2012</v>
       </c>
       <c r="D10" t="s">
         <v>50</v>
       </c>
-      <c r="E10">
-        <v>2011</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="G10">
-        <v>2012</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A11">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
         <v>52</v>
@@ -718,19 +761,10 @@
         <v>50</v>
       </c>
       <c r="E11">
-        <v>2018</v>
-      </c>
-      <c r="G11">
-        <v>2016</v>
-      </c>
-      <c r="I11">
-        <v>2013</v>
-      </c>
-      <c r="K11">
         <v>1999</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>0</v>
       </c>
@@ -750,7 +784,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>8</v>
       </c>
@@ -779,7 +813,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>9</v>
       </c>
@@ -790,7 +824,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>1</v>
       </c>
@@ -816,7 +850,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>10</v>
       </c>
@@ -1101,12 +1135,6 @@
       </c>
       <c r="C37">
         <v>2000</v>
-      </c>
-      <c r="E37">
-        <v>2019</v>
-      </c>
-      <c r="G37">
-        <v>2018</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.35">
@@ -1263,7 +1291,7 @@
   <dimension ref="A1:K40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1271,7 +1299,7 @@
     <col min="2" max="2" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -1279,7 +1307,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1311,7 +1339,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>2</v>
       </c>
@@ -1322,7 +1350,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>3</v>
       </c>
@@ -1336,7 +1364,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>5</v>
       </c>
@@ -1347,7 +1375,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>3</v>
       </c>
@@ -1373,7 +1401,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>7</v>
       </c>
@@ -1390,7 +1418,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
         <v>2</v>
       </c>
@@ -1409,16 +1437,10 @@
       <c r="F8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="G8">
-        <v>2012</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
         <v>52</v>
@@ -1430,19 +1452,10 @@
         <v>50</v>
       </c>
       <c r="E9">
-        <v>2018</v>
-      </c>
-      <c r="G9">
-        <v>2016</v>
-      </c>
-      <c r="I9">
-        <v>2013</v>
-      </c>
-      <c r="K9">
         <v>1999</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>0</v>
       </c>
@@ -1462,7 +1475,7 @@
         <v>2017</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>8</v>
       </c>
@@ -1491,7 +1504,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>9</v>
       </c>
@@ -1502,7 +1515,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1510,25 +1523,13 @@
         <v>55</v>
       </c>
       <c r="C13">
-        <v>2006</v>
+        <v>2012</v>
       </c>
       <c r="D13" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E13">
-        <v>2012</v>
-      </c>
-      <c r="F13" t="s">
-        <v>50</v>
-      </c>
-      <c r="G13">
-        <v>2019</v>
-      </c>
-      <c r="H13" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>10</v>
       </c>
@@ -1545,7 +1546,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -1565,7 +1566,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>12</v>
       </c>
@@ -1781,12 +1782,6 @@
       </c>
       <c r="C31">
         <v>2000</v>
-      </c>
-      <c r="E31">
-        <v>2019</v>
-      </c>
-      <c r="G31">
-        <v>2018</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
@@ -1916,10 +1911,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H26"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1927,7 +1922,7 @@
     <col min="3" max="3" width="17.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -1935,7 +1930,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>56</v>
       </c>
@@ -1957,8 +1952,11 @@
       <c r="G2" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B3" t="s">
         <v>46</v>
       </c>
@@ -1969,7 +1967,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B4" t="s">
         <v>46</v>
       </c>
@@ -1983,7 +1981,7 @@
         <v>2011</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B5" t="s">
         <v>46</v>
       </c>
@@ -1994,7 +1992,7 @@
         <v>2003</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B6" t="s">
         <v>46</v>
       </c>
@@ -2011,9 +2009,9 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A7">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>50</v>
@@ -2025,19 +2023,10 @@
         <v>2011</v>
       </c>
       <c r="E7">
-        <v>2018</v>
-      </c>
-      <c r="F7">
-        <v>2016</v>
-      </c>
-      <c r="G7">
-        <v>2013</v>
-      </c>
-      <c r="H7">
         <v>1999</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B8" t="s">
         <v>46</v>
       </c>
@@ -2051,7 +2040,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>2</v>
       </c>
@@ -2068,7 +2057,7 @@
         <v>2016</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>46</v>
       </c>
@@ -2082,7 +2071,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>46</v>
       </c>
@@ -2096,7 +2085,7 @@
         <v>2010</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2113,7 +2102,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2130,7 +2119,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2144,7 +2133,7 @@
         <v>2002</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2161,7 +2150,7 @@
         <v>2006</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2244,12 +2233,6 @@
       </c>
       <c r="D20">
         <v>2000</v>
-      </c>
-      <c r="E20">
-        <v>2019</v>
-      </c>
-      <c r="F20">
-        <v>2018</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -2355,12 +2338,540 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="17.1796875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>56</v>
+      </c>
+      <c r="B2" t="s">
+        <v>70</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3">
+        <v>2000</v>
+      </c>
+      <c r="E3">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>1992</v>
+      </c>
+      <c r="E4">
+        <v>1995</v>
+      </c>
+      <c r="F4">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>1999</v>
+      </c>
+      <c r="E5">
+        <v>2011</v>
+      </c>
+      <c r="F5">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>2</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D6">
+        <v>1995</v>
+      </c>
+      <c r="E6">
+        <v>2011</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>50</v>
+      </c>
+      <c r="C7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D7">
+        <v>2011</v>
+      </c>
+      <c r="E7">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8">
+        <v>2008</v>
+      </c>
+      <c r="E8">
+        <v>2012</v>
+      </c>
+      <c r="F8">
+        <v>2019</v>
+      </c>
+      <c r="G8">
+        <v>2006</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" t="s">
+        <v>55</v>
+      </c>
+      <c r="D9">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C10" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10">
+        <v>2000</v>
+      </c>
+      <c r="E10">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11">
+        <v>2000</v>
+      </c>
+      <c r="E11">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B12" t="s">
+        <v>46</v>
+      </c>
+      <c r="C12" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12">
+        <v>2000</v>
+      </c>
+      <c r="E12">
+        <v>2010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" t="s">
+        <v>46</v>
+      </c>
+      <c r="C14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14">
+        <v>2012</v>
+      </c>
+      <c r="E14">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A15">
+        <v>2</v>
+      </c>
+      <c r="B15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15">
+        <v>2010</v>
+      </c>
+      <c r="E15">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>24</v>
+      </c>
+      <c r="D16">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A17">
+        <v>1</v>
+      </c>
+      <c r="B17" t="s">
+        <v>46</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17">
+        <v>2009</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>29</v>
+      </c>
+      <c r="D18">
+        <v>2007</v>
+      </c>
+      <c r="E18">
+        <v>2011</v>
+      </c>
+      <c r="F18">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A19">
+        <v>3</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>58</v>
+      </c>
+      <c r="D19">
+        <v>2013</v>
+      </c>
+      <c r="E19">
+        <v>2004</v>
+      </c>
+      <c r="F19">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A21">
+        <v>2</v>
+      </c>
+      <c r="B21" t="s">
+        <v>46</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21">
+        <v>2003</v>
+      </c>
+      <c r="E21">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A22">
+        <v>2</v>
+      </c>
+      <c r="B22" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" t="s">
+        <v>38</v>
+      </c>
+      <c r="D22">
+        <v>2012</v>
+      </c>
+      <c r="E22">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A23">
+        <v>4</v>
+      </c>
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="D23">
+        <v>2019</v>
+      </c>
+      <c r="E23">
+        <v>2009</v>
+      </c>
+      <c r="F23">
+        <v>2012</v>
+      </c>
+      <c r="G23">
+        <v>2016</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" t="s">
+        <v>40</v>
+      </c>
+      <c r="D24">
+        <v>2012</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="17" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2">
+        <v>1996</v>
+      </c>
+      <c r="C2">
+        <v>2014</v>
+      </c>
+      <c r="H2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3">
+        <v>2000</v>
+      </c>
+      <c r="C3">
+        <v>2010</v>
+      </c>
+      <c r="H3" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B4">
+        <v>1993</v>
+      </c>
+      <c r="C4">
+        <v>2002</v>
+      </c>
+      <c r="D4">
+        <v>2005</v>
+      </c>
+      <c r="E4">
+        <v>2009</v>
+      </c>
+      <c r="H4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B5">
+        <v>1993</v>
+      </c>
+      <c r="C5">
+        <v>2002</v>
+      </c>
+      <c r="D5">
+        <v>2004</v>
+      </c>
+      <c r="E5">
+        <v>2006</v>
+      </c>
+      <c r="F5">
+        <v>2009</v>
+      </c>
+      <c r="H5" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B6">
+        <v>2010</v>
+      </c>
+      <c r="H6" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B7">
+        <v>2011</v>
+      </c>
+      <c r="H7" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>